<commit_message>
fix insert in xlsx
</commit_message>
<xml_diff>
--- a/template/Реестр заявок №327.xlsx
+++ b/template/Реестр заявок №327.xlsx
@@ -5,30 +5,22 @@
   <workbookPr codeName="ЭтаКнига" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Programmist\Anton\word_generator\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Programmist\Anton\word_generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9410"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Лист1!$A$1:$J$421</definedName>
-  </definedNames>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Дата поступления заявок</t>
   </si>
@@ -36,10 +28,13 @@
     <t>Количество поступивших заявок</t>
   </si>
   <si>
+    <t>№ п/п</t>
+  </si>
+  <si>
     <t>Наименование организации</t>
   </si>
   <si>
-    <t>№ п/п</t>
+    <t>ИНН организации</t>
   </si>
   <si>
     <t>№ заявки</t>
@@ -54,25 +49,34 @@
     <t>Дата передачи аналитическому отделу</t>
   </si>
   <si>
-    <t>ИНН организации</t>
+    <t>ФИО принявшего заявку в аналитическом отделе</t>
   </si>
   <si>
-    <t>ФИО принявшего заявку в аналитическом отделе</t>
+    <t>ООО "Мир Спорта"</t>
+  </si>
+  <si>
+    <t>1658148223</t>
+  </si>
+  <si>
+    <t>12.05.2020</t>
+  </si>
+  <si>
+    <t>Е.Р. Зотина</t>
   </si>
   <si>
     <t>Галиев М.Р.</t>
   </si>
   <si>
+    <t>Шайдуллина Д.Р.</t>
+  </si>
+  <si>
     <t>Соловьев Д.З.</t>
   </si>
   <si>
-    <t>Зотина Е.Р.</t>
+    <t>Бобиенко О.А.</t>
   </si>
   <si>
-    <t>Шайдуллина Д.Р.</t>
-  </si>
-  <si>
-    <t>Бобиенко О.А.</t>
+    <t>Зотина Е.Р.</t>
   </si>
   <si>
     <t>Гареев Р.М.</t>
@@ -80,12 +84,24 @@
   <si>
     <t>Сафин Р.Ф.</t>
   </si>
+  <si>
+    <t>без заключения</t>
+  </si>
+  <si>
+    <t>Шайдуллина Д.</t>
+  </si>
+  <si>
+    <t>итого:     1</t>
+  </si>
+  <si>
+    <t>П-120520201754</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -101,13 +117,29 @@
       <family val="1"/>
       <charset val="204"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="5">
@@ -178,7 +210,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -195,6 +227,13 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -476,26 +515,26 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Лист1"/>
-  <dimension ref="A1:J421"/>
+  <dimension ref="A1:K422"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:F421"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.90625" customWidth="1"/>
-    <col min="2" max="2" width="17.81640625" customWidth="1"/>
-    <col min="4" max="4" width="22.36328125" customWidth="1"/>
+    <col min="1" max="2" width="17.81640625" customWidth="1"/>
+    <col min="4" max="4" width="22.453125" customWidth="1"/>
     <col min="5" max="5" width="15.54296875" customWidth="1"/>
     <col min="6" max="6" width="18" customWidth="1"/>
-    <col min="7" max="7" width="16.90625" customWidth="1"/>
+    <col min="7" max="7" width="16.81640625" customWidth="1"/>
     <col min="8" max="8" width="13.1796875" customWidth="1"/>
-    <col min="9" max="9" width="17.90625" customWidth="1"/>
+    <col min="9" max="9" width="17.81640625" customWidth="1"/>
     <col min="10" max="10" width="18.54296875" customWidth="1"/>
+    <col min="11" max="11" width="20.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -503,63 +542,84 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>2</v>
-      </c>
       <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>7</v>
       </c>
       <c r="J1" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A2" s="7">
+        <v>43963</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
       <c r="C2" s="2">
         <v>1</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" s="6"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1">
-        <v>2</v>
-      </c>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4" s="1"/>
+      <c r="D2" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="7">
+        <v>43964</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="10"/>
+      <c r="B3" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="12"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="12"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A4" s="6"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
@@ -569,11 +629,11 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
@@ -583,11 +643,11 @@
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
@@ -597,11 +657,11 @@
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
@@ -611,11 +671,11 @@
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D8" s="9"/>
       <c r="E8" s="9"/>
@@ -625,11 +685,11 @@
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D9" s="9"/>
       <c r="E9" s="9"/>
@@ -639,11 +699,11 @@
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
@@ -653,11 +713,11 @@
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
@@ -667,11 +727,11 @@
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
@@ -681,11 +741,11 @@
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D13" s="9"/>
       <c r="E13" s="9"/>
@@ -695,11 +755,11 @@
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
@@ -709,11 +769,11 @@
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D15" s="9"/>
       <c r="E15" s="9"/>
@@ -723,11 +783,11 @@
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D16" s="9"/>
       <c r="E16" s="9"/>
@@ -741,7 +801,7 @@
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D17" s="9"/>
       <c r="E17" s="9"/>
@@ -755,7 +815,7 @@
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D18" s="9"/>
       <c r="E18" s="9"/>
@@ -769,7 +829,7 @@
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D19" s="9"/>
       <c r="E19" s="9"/>
@@ -783,7 +843,7 @@
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D20" s="9"/>
       <c r="E20" s="9"/>
@@ -797,7 +857,7 @@
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D21" s="9"/>
       <c r="E21" s="9"/>
@@ -811,7 +871,7 @@
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D22" s="9"/>
       <c r="E22" s="9"/>
@@ -825,7 +885,7 @@
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D23" s="9"/>
       <c r="E23" s="9"/>
@@ -839,7 +899,7 @@
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D24" s="9"/>
       <c r="E24" s="9"/>
@@ -853,7 +913,7 @@
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D25" s="9"/>
       <c r="E25" s="9"/>
@@ -867,7 +927,7 @@
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D26" s="9"/>
       <c r="E26" s="9"/>
@@ -881,7 +941,7 @@
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D27" s="9"/>
       <c r="E27" s="9"/>
@@ -895,7 +955,7 @@
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D28" s="9"/>
       <c r="E28" s="9"/>
@@ -909,7 +969,7 @@
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D29" s="9"/>
       <c r="E29" s="9"/>
@@ -923,7 +983,7 @@
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D30" s="9"/>
       <c r="E30" s="9"/>
@@ -937,7 +997,7 @@
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D31" s="9"/>
       <c r="E31" s="9"/>
@@ -951,7 +1011,7 @@
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D32" s="9"/>
       <c r="E32" s="9"/>
@@ -965,7 +1025,7 @@
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D33" s="9"/>
       <c r="E33" s="9"/>
@@ -979,7 +1039,7 @@
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D34" s="9"/>
       <c r="E34" s="9"/>
@@ -993,7 +1053,7 @@
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D35" s="9"/>
       <c r="E35" s="9"/>
@@ -1007,7 +1067,7 @@
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D36" s="9"/>
       <c r="E36" s="9"/>
@@ -1021,7 +1081,7 @@
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D37" s="9"/>
       <c r="E37" s="9"/>
@@ -1035,7 +1095,7 @@
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D38" s="9"/>
       <c r="E38" s="9"/>
@@ -1049,7 +1109,7 @@
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D39" s="9"/>
       <c r="E39" s="9"/>
@@ -1063,7 +1123,7 @@
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D40" s="9"/>
       <c r="E40" s="9"/>
@@ -1077,7 +1137,7 @@
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D41" s="9"/>
       <c r="E41" s="9"/>
@@ -1091,7 +1151,7 @@
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D42" s="9"/>
       <c r="E42" s="9"/>
@@ -1105,7 +1165,7 @@
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D43" s="9"/>
       <c r="E43" s="9"/>
@@ -1119,7 +1179,7 @@
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D44" s="9"/>
       <c r="E44" s="9"/>
@@ -1133,7 +1193,7 @@
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D45" s="9"/>
       <c r="E45" s="9"/>
@@ -1147,7 +1207,7 @@
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D46" s="9"/>
       <c r="E46" s="9"/>
@@ -1161,7 +1221,7 @@
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D47" s="9"/>
       <c r="E47" s="9"/>
@@ -1175,7 +1235,7 @@
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D48" s="9"/>
       <c r="E48" s="9"/>
@@ -1189,7 +1249,7 @@
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D49" s="9"/>
       <c r="E49" s="9"/>
@@ -1203,7 +1263,7 @@
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D50" s="9"/>
       <c r="E50" s="9"/>
@@ -1217,7 +1277,7 @@
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D51" s="9"/>
       <c r="E51" s="9"/>
@@ -1231,7 +1291,7 @@
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D52" s="9"/>
       <c r="E52" s="9"/>
@@ -1245,7 +1305,7 @@
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D53" s="9"/>
       <c r="E53" s="9"/>
@@ -1259,7 +1319,7 @@
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D54" s="9"/>
       <c r="E54" s="9"/>
@@ -1273,7 +1333,7 @@
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D55" s="9"/>
       <c r="E55" s="9"/>
@@ -1287,7 +1347,7 @@
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D56" s="9"/>
       <c r="E56" s="9"/>
@@ -1301,7 +1361,7 @@
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D57" s="9"/>
       <c r="E57" s="9"/>
@@ -1315,7 +1375,7 @@
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D58" s="9"/>
       <c r="E58" s="9"/>
@@ -1329,7 +1389,7 @@
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D59" s="9"/>
       <c r="E59" s="9"/>
@@ -1343,7 +1403,7 @@
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D60" s="9"/>
       <c r="E60" s="9"/>
@@ -1357,7 +1417,7 @@
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D61" s="9"/>
       <c r="E61" s="9"/>
@@ -1371,7 +1431,7 @@
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D62" s="9"/>
       <c r="E62" s="9"/>
@@ -1385,7 +1445,7 @@
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D63" s="9"/>
       <c r="E63" s="9"/>
@@ -1399,7 +1459,7 @@
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D64" s="9"/>
       <c r="E64" s="9"/>
@@ -1413,7 +1473,7 @@
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D65" s="9"/>
       <c r="E65" s="9"/>
@@ -1427,7 +1487,7 @@
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D66" s="9"/>
       <c r="E66" s="9"/>
@@ -1441,7 +1501,7 @@
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D67" s="9"/>
       <c r="E67" s="9"/>
@@ -1455,7 +1515,7 @@
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D68" s="9"/>
       <c r="E68" s="9"/>
@@ -1469,7 +1529,7 @@
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D69" s="9"/>
       <c r="E69" s="9"/>
@@ -1483,7 +1543,7 @@
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D70" s="9"/>
       <c r="E70" s="9"/>
@@ -1497,7 +1557,7 @@
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D71" s="9"/>
       <c r="E71" s="9"/>
@@ -1511,7 +1571,7 @@
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D72" s="9"/>
       <c r="E72" s="9"/>
@@ -1525,7 +1585,7 @@
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D73" s="9"/>
       <c r="E73" s="9"/>
@@ -1539,7 +1599,7 @@
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D74" s="9"/>
       <c r="E74" s="9"/>
@@ -1553,7 +1613,7 @@
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D75" s="9"/>
       <c r="E75" s="9"/>
@@ -1567,7 +1627,7 @@
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D76" s="9"/>
       <c r="E76" s="9"/>
@@ -1581,7 +1641,7 @@
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D77" s="9"/>
       <c r="E77" s="9"/>
@@ -1595,7 +1655,7 @@
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D78" s="9"/>
       <c r="E78" s="9"/>
@@ -1609,7 +1669,7 @@
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D79" s="9"/>
       <c r="E79" s="9"/>
@@ -1623,7 +1683,7 @@
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D80" s="9"/>
       <c r="E80" s="9"/>
@@ -1637,7 +1697,7 @@
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D81" s="9"/>
       <c r="E81" s="9"/>
@@ -1651,7 +1711,7 @@
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D82" s="9"/>
       <c r="E82" s="9"/>
@@ -1665,7 +1725,7 @@
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D83" s="9"/>
       <c r="E83" s="9"/>
@@ -1679,7 +1739,7 @@
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D84" s="9"/>
       <c r="E84" s="9"/>
@@ -1693,7 +1753,7 @@
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D85" s="9"/>
       <c r="E85" s="9"/>
@@ -1707,7 +1767,7 @@
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D86" s="9"/>
       <c r="E86" s="9"/>
@@ -1721,7 +1781,7 @@
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D87" s="9"/>
       <c r="E87" s="9"/>
@@ -1735,7 +1795,7 @@
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D88" s="9"/>
       <c r="E88" s="9"/>
@@ -1749,7 +1809,7 @@
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D89" s="9"/>
       <c r="E89" s="9"/>
@@ -1763,7 +1823,7 @@
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D90" s="9"/>
       <c r="E90" s="9"/>
@@ -1777,7 +1837,7 @@
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D91" s="9"/>
       <c r="E91" s="9"/>
@@ -1791,7 +1851,7 @@
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D92" s="9"/>
       <c r="E92" s="9"/>
@@ -1805,7 +1865,7 @@
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D93" s="9"/>
       <c r="E93" s="9"/>
@@ -1819,7 +1879,7 @@
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D94" s="9"/>
       <c r="E94" s="9"/>
@@ -1833,7 +1893,7 @@
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D95" s="9"/>
       <c r="E95" s="9"/>
@@ -1847,7 +1907,7 @@
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D96" s="9"/>
       <c r="E96" s="9"/>
@@ -1861,7 +1921,7 @@
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D97" s="9"/>
       <c r="E97" s="9"/>
@@ -1875,7 +1935,7 @@
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D98" s="9"/>
       <c r="E98" s="9"/>
@@ -1889,7 +1949,7 @@
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D99" s="9"/>
       <c r="E99" s="9"/>
@@ -1903,7 +1963,7 @@
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D100" s="9"/>
       <c r="E100" s="9"/>
@@ -1917,7 +1977,7 @@
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
       <c r="C101" s="1">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D101" s="9"/>
       <c r="E101" s="9"/>
@@ -1931,7 +1991,7 @@
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D102" s="9"/>
       <c r="E102" s="9"/>
@@ -1945,7 +2005,7 @@
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
       <c r="C103" s="1">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D103" s="9"/>
       <c r="E103" s="9"/>
@@ -1959,7 +2019,7 @@
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
       <c r="C104" s="1">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D104" s="9"/>
       <c r="E104" s="9"/>
@@ -1973,7 +2033,7 @@
       <c r="A105" s="1"/>
       <c r="B105" s="1"/>
       <c r="C105" s="1">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D105" s="9"/>
       <c r="E105" s="9"/>
@@ -1987,7 +2047,7 @@
       <c r="A106" s="1"/>
       <c r="B106" s="1"/>
       <c r="C106" s="1">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D106" s="9"/>
       <c r="E106" s="9"/>
@@ -2001,7 +2061,7 @@
       <c r="A107" s="1"/>
       <c r="B107" s="1"/>
       <c r="C107" s="1">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D107" s="9"/>
       <c r="E107" s="9"/>
@@ -2015,7 +2075,7 @@
       <c r="A108" s="1"/>
       <c r="B108" s="1"/>
       <c r="C108" s="1">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D108" s="9"/>
       <c r="E108" s="9"/>
@@ -2029,7 +2089,7 @@
       <c r="A109" s="1"/>
       <c r="B109" s="1"/>
       <c r="C109" s="1">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D109" s="9"/>
       <c r="E109" s="9"/>
@@ -2043,7 +2103,7 @@
       <c r="A110" s="1"/>
       <c r="B110" s="1"/>
       <c r="C110" s="1">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D110" s="9"/>
       <c r="E110" s="9"/>
@@ -2057,7 +2117,7 @@
       <c r="A111" s="1"/>
       <c r="B111" s="1"/>
       <c r="C111" s="1">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D111" s="9"/>
       <c r="E111" s="9"/>
@@ -2071,7 +2131,7 @@
       <c r="A112" s="1"/>
       <c r="B112" s="1"/>
       <c r="C112" s="1">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D112" s="9"/>
       <c r="E112" s="9"/>
@@ -2085,7 +2145,7 @@
       <c r="A113" s="1"/>
       <c r="B113" s="1"/>
       <c r="C113" s="1">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D113" s="9"/>
       <c r="E113" s="9"/>
@@ -2099,7 +2159,7 @@
       <c r="A114" s="1"/>
       <c r="B114" s="1"/>
       <c r="C114" s="1">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D114" s="9"/>
       <c r="E114" s="9"/>
@@ -2113,7 +2173,7 @@
       <c r="A115" s="1"/>
       <c r="B115" s="1"/>
       <c r="C115" s="1">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D115" s="9"/>
       <c r="E115" s="9"/>
@@ -2127,7 +2187,7 @@
       <c r="A116" s="1"/>
       <c r="B116" s="1"/>
       <c r="C116" s="1">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D116" s="9"/>
       <c r="E116" s="9"/>
@@ -2141,7 +2201,7 @@
       <c r="A117" s="1"/>
       <c r="B117" s="1"/>
       <c r="C117" s="1">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D117" s="9"/>
       <c r="E117" s="9"/>
@@ -2155,7 +2215,7 @@
       <c r="A118" s="1"/>
       <c r="B118" s="1"/>
       <c r="C118" s="1">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D118" s="9"/>
       <c r="E118" s="9"/>
@@ -2169,7 +2229,7 @@
       <c r="A119" s="1"/>
       <c r="B119" s="1"/>
       <c r="C119" s="1">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D119" s="9"/>
       <c r="E119" s="9"/>
@@ -2183,7 +2243,7 @@
       <c r="A120" s="1"/>
       <c r="B120" s="1"/>
       <c r="C120" s="1">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D120" s="9"/>
       <c r="E120" s="9"/>
@@ -2197,7 +2257,7 @@
       <c r="A121" s="1"/>
       <c r="B121" s="1"/>
       <c r="C121" s="1">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D121" s="9"/>
       <c r="E121" s="9"/>
@@ -2211,7 +2271,7 @@
       <c r="A122" s="1"/>
       <c r="B122" s="1"/>
       <c r="C122" s="1">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D122" s="9"/>
       <c r="E122" s="9"/>
@@ -2225,7 +2285,7 @@
       <c r="A123" s="1"/>
       <c r="B123" s="1"/>
       <c r="C123" s="1">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D123" s="9"/>
       <c r="E123" s="9"/>
@@ -2239,7 +2299,7 @@
       <c r="A124" s="1"/>
       <c r="B124" s="1"/>
       <c r="C124" s="1">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D124" s="9"/>
       <c r="E124" s="9"/>
@@ -2253,7 +2313,7 @@
       <c r="A125" s="1"/>
       <c r="B125" s="1"/>
       <c r="C125" s="1">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D125" s="9"/>
       <c r="E125" s="9"/>
@@ -2267,7 +2327,7 @@
       <c r="A126" s="1"/>
       <c r="B126" s="1"/>
       <c r="C126" s="1">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D126" s="9"/>
       <c r="E126" s="9"/>
@@ -2281,7 +2341,7 @@
       <c r="A127" s="1"/>
       <c r="B127" s="1"/>
       <c r="C127" s="1">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D127" s="9"/>
       <c r="E127" s="9"/>
@@ -2295,7 +2355,7 @@
       <c r="A128" s="1"/>
       <c r="B128" s="1"/>
       <c r="C128" s="1">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D128" s="9"/>
       <c r="E128" s="9"/>
@@ -2309,7 +2369,7 @@
       <c r="A129" s="1"/>
       <c r="B129" s="1"/>
       <c r="C129" s="1">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D129" s="9"/>
       <c r="E129" s="9"/>
@@ -2323,7 +2383,7 @@
       <c r="A130" s="1"/>
       <c r="B130" s="1"/>
       <c r="C130" s="1">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D130" s="9"/>
       <c r="E130" s="9"/>
@@ -2337,7 +2397,7 @@
       <c r="A131" s="1"/>
       <c r="B131" s="1"/>
       <c r="C131" s="1">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D131" s="9"/>
       <c r="E131" s="9"/>
@@ -2351,7 +2411,7 @@
       <c r="A132" s="1"/>
       <c r="B132" s="1"/>
       <c r="C132" s="1">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D132" s="9"/>
       <c r="E132" s="9"/>
@@ -2365,7 +2425,7 @@
       <c r="A133" s="1"/>
       <c r="B133" s="1"/>
       <c r="C133" s="1">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D133" s="9"/>
       <c r="E133" s="9"/>
@@ -2379,7 +2439,7 @@
       <c r="A134" s="1"/>
       <c r="B134" s="1"/>
       <c r="C134" s="1">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D134" s="9"/>
       <c r="E134" s="9"/>
@@ -2393,7 +2453,7 @@
       <c r="A135" s="1"/>
       <c r="B135" s="1"/>
       <c r="C135" s="1">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D135" s="9"/>
       <c r="E135" s="9"/>
@@ -2407,7 +2467,7 @@
       <c r="A136" s="1"/>
       <c r="B136" s="1"/>
       <c r="C136" s="1">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D136" s="9"/>
       <c r="E136" s="9"/>
@@ -2421,7 +2481,7 @@
       <c r="A137" s="1"/>
       <c r="B137" s="1"/>
       <c r="C137" s="1">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D137" s="9"/>
       <c r="E137" s="9"/>
@@ -2435,7 +2495,7 @@
       <c r="A138" s="1"/>
       <c r="B138" s="1"/>
       <c r="C138" s="1">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D138" s="9"/>
       <c r="E138" s="9"/>
@@ -2449,7 +2509,7 @@
       <c r="A139" s="1"/>
       <c r="B139" s="1"/>
       <c r="C139" s="1">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D139" s="9"/>
       <c r="E139" s="9"/>
@@ -2463,7 +2523,7 @@
       <c r="A140" s="1"/>
       <c r="B140" s="1"/>
       <c r="C140" s="1">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D140" s="9"/>
       <c r="E140" s="9"/>
@@ -2477,7 +2537,7 @@
       <c r="A141" s="1"/>
       <c r="B141" s="1"/>
       <c r="C141" s="1">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D141" s="9"/>
       <c r="E141" s="9"/>
@@ -2491,7 +2551,7 @@
       <c r="A142" s="1"/>
       <c r="B142" s="1"/>
       <c r="C142" s="1">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D142" s="9"/>
       <c r="E142" s="9"/>
@@ -2505,7 +2565,7 @@
       <c r="A143" s="1"/>
       <c r="B143" s="1"/>
       <c r="C143" s="1">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D143" s="9"/>
       <c r="E143" s="9"/>
@@ -2519,7 +2579,7 @@
       <c r="A144" s="1"/>
       <c r="B144" s="1"/>
       <c r="C144" s="1">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D144" s="9"/>
       <c r="E144" s="9"/>
@@ -2533,7 +2593,7 @@
       <c r="A145" s="1"/>
       <c r="B145" s="1"/>
       <c r="C145" s="1">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D145" s="9"/>
       <c r="E145" s="9"/>
@@ -2547,7 +2607,7 @@
       <c r="A146" s="1"/>
       <c r="B146" s="1"/>
       <c r="C146" s="1">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D146" s="9"/>
       <c r="E146" s="9"/>
@@ -2561,7 +2621,7 @@
       <c r="A147" s="1"/>
       <c r="B147" s="1"/>
       <c r="C147" s="1">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D147" s="9"/>
       <c r="E147" s="9"/>
@@ -2575,7 +2635,7 @@
       <c r="A148" s="1"/>
       <c r="B148" s="1"/>
       <c r="C148" s="1">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D148" s="9"/>
       <c r="E148" s="9"/>
@@ -2589,7 +2649,7 @@
       <c r="A149" s="1"/>
       <c r="B149" s="1"/>
       <c r="C149" s="1">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D149" s="9"/>
       <c r="E149" s="9"/>
@@ -2603,7 +2663,7 @@
       <c r="A150" s="1"/>
       <c r="B150" s="1"/>
       <c r="C150" s="1">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D150" s="9"/>
       <c r="E150" s="9"/>
@@ -2617,7 +2677,7 @@
       <c r="A151" s="1"/>
       <c r="B151" s="1"/>
       <c r="C151" s="1">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D151" s="9"/>
       <c r="E151" s="9"/>
@@ -2631,7 +2691,7 @@
       <c r="A152" s="1"/>
       <c r="B152" s="1"/>
       <c r="C152" s="1">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D152" s="9"/>
       <c r="E152" s="9"/>
@@ -2645,7 +2705,7 @@
       <c r="A153" s="1"/>
       <c r="B153" s="1"/>
       <c r="C153" s="1">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D153" s="9"/>
       <c r="E153" s="9"/>
@@ -2659,7 +2719,7 @@
       <c r="A154" s="1"/>
       <c r="B154" s="1"/>
       <c r="C154" s="1">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D154" s="9"/>
       <c r="E154" s="9"/>
@@ -2673,7 +2733,7 @@
       <c r="A155" s="1"/>
       <c r="B155" s="1"/>
       <c r="C155" s="1">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D155" s="9"/>
       <c r="E155" s="9"/>
@@ -2687,7 +2747,7 @@
       <c r="A156" s="1"/>
       <c r="B156" s="1"/>
       <c r="C156" s="1">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D156" s="9"/>
       <c r="E156" s="9"/>
@@ -2701,7 +2761,7 @@
       <c r="A157" s="1"/>
       <c r="B157" s="1"/>
       <c r="C157" s="1">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D157" s="9"/>
       <c r="E157" s="9"/>
@@ -2715,7 +2775,7 @@
       <c r="A158" s="1"/>
       <c r="B158" s="1"/>
       <c r="C158" s="1">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D158" s="9"/>
       <c r="E158" s="9"/>
@@ -2729,7 +2789,7 @@
       <c r="A159" s="1"/>
       <c r="B159" s="1"/>
       <c r="C159" s="1">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D159" s="9"/>
       <c r="E159" s="9"/>
@@ -2743,7 +2803,7 @@
       <c r="A160" s="1"/>
       <c r="B160" s="1"/>
       <c r="C160" s="1">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D160" s="9"/>
       <c r="E160" s="9"/>
@@ -2757,7 +2817,7 @@
       <c r="A161" s="1"/>
       <c r="B161" s="1"/>
       <c r="C161" s="1">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D161" s="9"/>
       <c r="E161" s="9"/>
@@ -2771,7 +2831,7 @@
       <c r="A162" s="1"/>
       <c r="B162" s="1"/>
       <c r="C162" s="1">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D162" s="9"/>
       <c r="E162" s="9"/>
@@ -2785,7 +2845,7 @@
       <c r="A163" s="1"/>
       <c r="B163" s="1"/>
       <c r="C163" s="1">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D163" s="9"/>
       <c r="E163" s="9"/>
@@ -2799,7 +2859,7 @@
       <c r="A164" s="1"/>
       <c r="B164" s="1"/>
       <c r="C164" s="1">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D164" s="9"/>
       <c r="E164" s="9"/>
@@ -2813,7 +2873,7 @@
       <c r="A165" s="1"/>
       <c r="B165" s="1"/>
       <c r="C165" s="1">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D165" s="9"/>
       <c r="E165" s="9"/>
@@ -2827,7 +2887,7 @@
       <c r="A166" s="1"/>
       <c r="B166" s="1"/>
       <c r="C166" s="1">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D166" s="9"/>
       <c r="E166" s="9"/>
@@ -2841,7 +2901,7 @@
       <c r="A167" s="1"/>
       <c r="B167" s="1"/>
       <c r="C167" s="1">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D167" s="9"/>
       <c r="E167" s="9"/>
@@ -2855,7 +2915,7 @@
       <c r="A168" s="1"/>
       <c r="B168" s="1"/>
       <c r="C168" s="1">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D168" s="9"/>
       <c r="E168" s="9"/>
@@ -2869,7 +2929,7 @@
       <c r="A169" s="1"/>
       <c r="B169" s="1"/>
       <c r="C169" s="1">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D169" s="9"/>
       <c r="E169" s="9"/>
@@ -2883,7 +2943,7 @@
       <c r="A170" s="1"/>
       <c r="B170" s="1"/>
       <c r="C170" s="1">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D170" s="9"/>
       <c r="E170" s="9"/>
@@ -2897,7 +2957,7 @@
       <c r="A171" s="1"/>
       <c r="B171" s="1"/>
       <c r="C171" s="1">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D171" s="9"/>
       <c r="E171" s="9"/>
@@ -2911,7 +2971,7 @@
       <c r="A172" s="1"/>
       <c r="B172" s="1"/>
       <c r="C172" s="1">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D172" s="9"/>
       <c r="E172" s="9"/>
@@ -2925,7 +2985,7 @@
       <c r="A173" s="1"/>
       <c r="B173" s="1"/>
       <c r="C173" s="1">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D173" s="9"/>
       <c r="E173" s="9"/>
@@ -2939,7 +2999,7 @@
       <c r="A174" s="1"/>
       <c r="B174" s="1"/>
       <c r="C174" s="1">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D174" s="9"/>
       <c r="E174" s="9"/>
@@ -2953,7 +3013,7 @@
       <c r="A175" s="1"/>
       <c r="B175" s="1"/>
       <c r="C175" s="1">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D175" s="9"/>
       <c r="E175" s="9"/>
@@ -2967,7 +3027,7 @@
       <c r="A176" s="1"/>
       <c r="B176" s="1"/>
       <c r="C176" s="1">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D176" s="9"/>
       <c r="E176" s="9"/>
@@ -2981,7 +3041,7 @@
       <c r="A177" s="1"/>
       <c r="B177" s="1"/>
       <c r="C177" s="1">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D177" s="9"/>
       <c r="E177" s="9"/>
@@ -2995,7 +3055,7 @@
       <c r="A178" s="1"/>
       <c r="B178" s="1"/>
       <c r="C178" s="1">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D178" s="9"/>
       <c r="E178" s="9"/>
@@ -3009,7 +3069,7 @@
       <c r="A179" s="1"/>
       <c r="B179" s="1"/>
       <c r="C179" s="1">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D179" s="9"/>
       <c r="E179" s="9"/>
@@ -3023,7 +3083,7 @@
       <c r="A180" s="1"/>
       <c r="B180" s="1"/>
       <c r="C180" s="1">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D180" s="9"/>
       <c r="E180" s="9"/>
@@ -3037,7 +3097,7 @@
       <c r="A181" s="1"/>
       <c r="B181" s="1"/>
       <c r="C181" s="1">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D181" s="9"/>
       <c r="E181" s="9"/>
@@ -3051,7 +3111,7 @@
       <c r="A182" s="1"/>
       <c r="B182" s="1"/>
       <c r="C182" s="1">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D182" s="9"/>
       <c r="E182" s="9"/>
@@ -3065,7 +3125,7 @@
       <c r="A183" s="1"/>
       <c r="B183" s="1"/>
       <c r="C183" s="1">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D183" s="9"/>
       <c r="E183" s="9"/>
@@ -3079,7 +3139,7 @@
       <c r="A184" s="1"/>
       <c r="B184" s="1"/>
       <c r="C184" s="1">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D184" s="9"/>
       <c r="E184" s="9"/>
@@ -3093,7 +3153,7 @@
       <c r="A185" s="1"/>
       <c r="B185" s="1"/>
       <c r="C185" s="1">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D185" s="9"/>
       <c r="E185" s="9"/>
@@ -3107,7 +3167,7 @@
       <c r="A186" s="1"/>
       <c r="B186" s="1"/>
       <c r="C186" s="1">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D186" s="9"/>
       <c r="E186" s="9"/>
@@ -3121,7 +3181,7 @@
       <c r="A187" s="1"/>
       <c r="B187" s="1"/>
       <c r="C187" s="1">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D187" s="9"/>
       <c r="E187" s="9"/>
@@ -3135,7 +3195,7 @@
       <c r="A188" s="1"/>
       <c r="B188" s="1"/>
       <c r="C188" s="1">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D188" s="9"/>
       <c r="E188" s="9"/>
@@ -3149,7 +3209,7 @@
       <c r="A189" s="1"/>
       <c r="B189" s="1"/>
       <c r="C189" s="1">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D189" s="9"/>
       <c r="E189" s="9"/>
@@ -3163,7 +3223,7 @@
       <c r="A190" s="1"/>
       <c r="B190" s="1"/>
       <c r="C190" s="1">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D190" s="9"/>
       <c r="E190" s="9"/>
@@ -3177,7 +3237,7 @@
       <c r="A191" s="1"/>
       <c r="B191" s="1"/>
       <c r="C191" s="1">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D191" s="9"/>
       <c r="E191" s="9"/>
@@ -3191,7 +3251,7 @@
       <c r="A192" s="1"/>
       <c r="B192" s="1"/>
       <c r="C192" s="1">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D192" s="9"/>
       <c r="E192" s="9"/>
@@ -3205,7 +3265,7 @@
       <c r="A193" s="1"/>
       <c r="B193" s="1"/>
       <c r="C193" s="1">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D193" s="9"/>
       <c r="E193" s="9"/>
@@ -3219,7 +3279,7 @@
       <c r="A194" s="1"/>
       <c r="B194" s="1"/>
       <c r="C194" s="1">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D194" s="9"/>
       <c r="E194" s="9"/>
@@ -3233,7 +3293,7 @@
       <c r="A195" s="1"/>
       <c r="B195" s="1"/>
       <c r="C195" s="1">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D195" s="9"/>
       <c r="E195" s="9"/>
@@ -3247,7 +3307,7 @@
       <c r="A196" s="1"/>
       <c r="B196" s="1"/>
       <c r="C196" s="1">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D196" s="9"/>
       <c r="E196" s="9"/>
@@ -3261,7 +3321,7 @@
       <c r="A197" s="1"/>
       <c r="B197" s="1"/>
       <c r="C197" s="1">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D197" s="9"/>
       <c r="E197" s="9"/>
@@ -3275,7 +3335,7 @@
       <c r="A198" s="1"/>
       <c r="B198" s="1"/>
       <c r="C198" s="1">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D198" s="9"/>
       <c r="E198" s="9"/>
@@ -3289,7 +3349,7 @@
       <c r="A199" s="1"/>
       <c r="B199" s="1"/>
       <c r="C199" s="1">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D199" s="9"/>
       <c r="E199" s="9"/>
@@ -3303,7 +3363,7 @@
       <c r="A200" s="1"/>
       <c r="B200" s="1"/>
       <c r="C200" s="1">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D200" s="9"/>
       <c r="E200" s="9"/>
@@ -3317,7 +3377,7 @@
       <c r="A201" s="1"/>
       <c r="B201" s="1"/>
       <c r="C201" s="1">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D201" s="9"/>
       <c r="E201" s="9"/>
@@ -3331,7 +3391,7 @@
       <c r="A202" s="1"/>
       <c r="B202" s="1"/>
       <c r="C202" s="1">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D202" s="9"/>
       <c r="E202" s="9"/>
@@ -3345,7 +3405,7 @@
       <c r="A203" s="1"/>
       <c r="B203" s="1"/>
       <c r="C203" s="1">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D203" s="9"/>
       <c r="E203" s="9"/>
@@ -3359,7 +3419,7 @@
       <c r="A204" s="1"/>
       <c r="B204" s="1"/>
       <c r="C204" s="1">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D204" s="9"/>
       <c r="E204" s="9"/>
@@ -3373,7 +3433,7 @@
       <c r="A205" s="1"/>
       <c r="B205" s="1"/>
       <c r="C205" s="1">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D205" s="9"/>
       <c r="E205" s="9"/>
@@ -3387,7 +3447,7 @@
       <c r="A206" s="1"/>
       <c r="B206" s="1"/>
       <c r="C206" s="1">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D206" s="9"/>
       <c r="E206" s="9"/>
@@ -3401,7 +3461,7 @@
       <c r="A207" s="1"/>
       <c r="B207" s="1"/>
       <c r="C207" s="1">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D207" s="9"/>
       <c r="E207" s="9"/>
@@ -3415,7 +3475,7 @@
       <c r="A208" s="1"/>
       <c r="B208" s="1"/>
       <c r="C208" s="1">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D208" s="9"/>
       <c r="E208" s="9"/>
@@ -3429,7 +3489,7 @@
       <c r="A209" s="1"/>
       <c r="B209" s="1"/>
       <c r="C209" s="1">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D209" s="9"/>
       <c r="E209" s="9"/>
@@ -3443,7 +3503,7 @@
       <c r="A210" s="1"/>
       <c r="B210" s="1"/>
       <c r="C210" s="1">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D210" s="9"/>
       <c r="E210" s="9"/>
@@ -3457,7 +3517,7 @@
       <c r="A211" s="1"/>
       <c r="B211" s="1"/>
       <c r="C211" s="1">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D211" s="9"/>
       <c r="E211" s="9"/>
@@ -3471,7 +3531,7 @@
       <c r="A212" s="1"/>
       <c r="B212" s="1"/>
       <c r="C212" s="1">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D212" s="9"/>
       <c r="E212" s="9"/>
@@ -3485,7 +3545,7 @@
       <c r="A213" s="1"/>
       <c r="B213" s="1"/>
       <c r="C213" s="1">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D213" s="9"/>
       <c r="E213" s="9"/>
@@ -3499,7 +3559,7 @@
       <c r="A214" s="1"/>
       <c r="B214" s="1"/>
       <c r="C214" s="1">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D214" s="9"/>
       <c r="E214" s="9"/>
@@ -3513,7 +3573,7 @@
       <c r="A215" s="1"/>
       <c r="B215" s="1"/>
       <c r="C215" s="1">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D215" s="9"/>
       <c r="E215" s="9"/>
@@ -3527,7 +3587,7 @@
       <c r="A216" s="1"/>
       <c r="B216" s="1"/>
       <c r="C216" s="1">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D216" s="9"/>
       <c r="E216" s="9"/>
@@ -3541,7 +3601,7 @@
       <c r="A217" s="1"/>
       <c r="B217" s="1"/>
       <c r="C217" s="1">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D217" s="9"/>
       <c r="E217" s="9"/>
@@ -3555,7 +3615,7 @@
       <c r="A218" s="1"/>
       <c r="B218" s="1"/>
       <c r="C218" s="1">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D218" s="9"/>
       <c r="E218" s="9"/>
@@ -3569,7 +3629,7 @@
       <c r="A219" s="1"/>
       <c r="B219" s="1"/>
       <c r="C219" s="1">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D219" s="9"/>
       <c r="E219" s="9"/>
@@ -3583,7 +3643,7 @@
       <c r="A220" s="1"/>
       <c r="B220" s="1"/>
       <c r="C220" s="1">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D220" s="9"/>
       <c r="E220" s="9"/>
@@ -3597,7 +3657,7 @@
       <c r="A221" s="1"/>
       <c r="B221" s="1"/>
       <c r="C221" s="1">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D221" s="9"/>
       <c r="E221" s="9"/>
@@ -3611,7 +3671,7 @@
       <c r="A222" s="1"/>
       <c r="B222" s="1"/>
       <c r="C222" s="1">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D222" s="9"/>
       <c r="E222" s="9"/>
@@ -3625,7 +3685,7 @@
       <c r="A223" s="1"/>
       <c r="B223" s="1"/>
       <c r="C223" s="1">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D223" s="9"/>
       <c r="E223" s="9"/>
@@ -3639,7 +3699,7 @@
       <c r="A224" s="1"/>
       <c r="B224" s="1"/>
       <c r="C224" s="1">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D224" s="9"/>
       <c r="E224" s="9"/>
@@ -3653,7 +3713,7 @@
       <c r="A225" s="1"/>
       <c r="B225" s="1"/>
       <c r="C225" s="1">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D225" s="9"/>
       <c r="E225" s="9"/>
@@ -3667,7 +3727,7 @@
       <c r="A226" s="1"/>
       <c r="B226" s="1"/>
       <c r="C226" s="1">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D226" s="9"/>
       <c r="E226" s="9"/>
@@ -3681,7 +3741,7 @@
       <c r="A227" s="1"/>
       <c r="B227" s="1"/>
       <c r="C227" s="1">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D227" s="9"/>
       <c r="E227" s="9"/>
@@ -3695,7 +3755,7 @@
       <c r="A228" s="1"/>
       <c r="B228" s="1"/>
       <c r="C228" s="1">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D228" s="9"/>
       <c r="E228" s="9"/>
@@ -3709,7 +3769,7 @@
       <c r="A229" s="1"/>
       <c r="B229" s="1"/>
       <c r="C229" s="1">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D229" s="9"/>
       <c r="E229" s="9"/>
@@ -3723,7 +3783,7 @@
       <c r="A230" s="1"/>
       <c r="B230" s="1"/>
       <c r="C230" s="1">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D230" s="9"/>
       <c r="E230" s="9"/>
@@ -3737,7 +3797,7 @@
       <c r="A231" s="1"/>
       <c r="B231" s="1"/>
       <c r="C231" s="1">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D231" s="9"/>
       <c r="E231" s="9"/>
@@ -3751,7 +3811,7 @@
       <c r="A232" s="1"/>
       <c r="B232" s="1"/>
       <c r="C232" s="1">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D232" s="9"/>
       <c r="E232" s="9"/>
@@ -3765,7 +3825,7 @@
       <c r="A233" s="1"/>
       <c r="B233" s="1"/>
       <c r="C233" s="1">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D233" s="9"/>
       <c r="E233" s="9"/>
@@ -3779,7 +3839,7 @@
       <c r="A234" s="1"/>
       <c r="B234" s="1"/>
       <c r="C234" s="1">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D234" s="9"/>
       <c r="E234" s="9"/>
@@ -3793,7 +3853,7 @@
       <c r="A235" s="1"/>
       <c r="B235" s="1"/>
       <c r="C235" s="1">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D235" s="9"/>
       <c r="E235" s="9"/>
@@ -3807,7 +3867,7 @@
       <c r="A236" s="1"/>
       <c r="B236" s="1"/>
       <c r="C236" s="1">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D236" s="9"/>
       <c r="E236" s="9"/>
@@ -3821,7 +3881,7 @@
       <c r="A237" s="1"/>
       <c r="B237" s="1"/>
       <c r="C237" s="1">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D237" s="9"/>
       <c r="E237" s="9"/>
@@ -3835,7 +3895,7 @@
       <c r="A238" s="1"/>
       <c r="B238" s="1"/>
       <c r="C238" s="1">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D238" s="9"/>
       <c r="E238" s="9"/>
@@ -3849,7 +3909,7 @@
       <c r="A239" s="1"/>
       <c r="B239" s="1"/>
       <c r="C239" s="1">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D239" s="9"/>
       <c r="E239" s="9"/>
@@ -3863,7 +3923,7 @@
       <c r="A240" s="1"/>
       <c r="B240" s="1"/>
       <c r="C240" s="1">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D240" s="9"/>
       <c r="E240" s="9"/>
@@ -3877,7 +3937,7 @@
       <c r="A241" s="1"/>
       <c r="B241" s="1"/>
       <c r="C241" s="1">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D241" s="9"/>
       <c r="E241" s="9"/>
@@ -3891,7 +3951,7 @@
       <c r="A242" s="1"/>
       <c r="B242" s="1"/>
       <c r="C242" s="1">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D242" s="9"/>
       <c r="E242" s="9"/>
@@ -3905,7 +3965,7 @@
       <c r="A243" s="1"/>
       <c r="B243" s="1"/>
       <c r="C243" s="1">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D243" s="9"/>
       <c r="E243" s="9"/>
@@ -3919,7 +3979,7 @@
       <c r="A244" s="1"/>
       <c r="B244" s="1"/>
       <c r="C244" s="1">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D244" s="9"/>
       <c r="E244" s="9"/>
@@ -3933,7 +3993,7 @@
       <c r="A245" s="1"/>
       <c r="B245" s="1"/>
       <c r="C245" s="1">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D245" s="9"/>
       <c r="E245" s="9"/>
@@ -3947,7 +4007,7 @@
       <c r="A246" s="1"/>
       <c r="B246" s="1"/>
       <c r="C246" s="1">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D246" s="9"/>
       <c r="E246" s="9"/>
@@ -3961,7 +4021,7 @@
       <c r="A247" s="1"/>
       <c r="B247" s="1"/>
       <c r="C247" s="1">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D247" s="9"/>
       <c r="E247" s="9"/>
@@ -3975,7 +4035,7 @@
       <c r="A248" s="1"/>
       <c r="B248" s="1"/>
       <c r="C248" s="1">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D248" s="9"/>
       <c r="E248" s="9"/>
@@ -3989,7 +4049,7 @@
       <c r="A249" s="1"/>
       <c r="B249" s="1"/>
       <c r="C249" s="1">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D249" s="9"/>
       <c r="E249" s="9"/>
@@ -4003,7 +4063,7 @@
       <c r="A250" s="1"/>
       <c r="B250" s="1"/>
       <c r="C250" s="1">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D250" s="9"/>
       <c r="E250" s="9"/>
@@ -4017,7 +4077,7 @@
       <c r="A251" s="1"/>
       <c r="B251" s="1"/>
       <c r="C251" s="1">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D251" s="9"/>
       <c r="E251" s="9"/>
@@ -4031,7 +4091,7 @@
       <c r="A252" s="1"/>
       <c r="B252" s="1"/>
       <c r="C252" s="1">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D252" s="9"/>
       <c r="E252" s="9"/>
@@ -4045,7 +4105,7 @@
       <c r="A253" s="1"/>
       <c r="B253" s="1"/>
       <c r="C253" s="1">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D253" s="9"/>
       <c r="E253" s="9"/>
@@ -4059,7 +4119,7 @@
       <c r="A254" s="1"/>
       <c r="B254" s="1"/>
       <c r="C254" s="1">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D254" s="9"/>
       <c r="E254" s="9"/>
@@ -4073,7 +4133,7 @@
       <c r="A255" s="1"/>
       <c r="B255" s="1"/>
       <c r="C255" s="1">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D255" s="9"/>
       <c r="E255" s="9"/>
@@ -4087,7 +4147,7 @@
       <c r="A256" s="1"/>
       <c r="B256" s="1"/>
       <c r="C256" s="1">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D256" s="9"/>
       <c r="E256" s="9"/>
@@ -4101,7 +4161,7 @@
       <c r="A257" s="1"/>
       <c r="B257" s="1"/>
       <c r="C257" s="1">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D257" s="9"/>
       <c r="E257" s="9"/>
@@ -4115,7 +4175,7 @@
       <c r="A258" s="1"/>
       <c r="B258" s="1"/>
       <c r="C258" s="1">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D258" s="9"/>
       <c r="E258" s="9"/>
@@ -4129,7 +4189,7 @@
       <c r="A259" s="1"/>
       <c r="B259" s="1"/>
       <c r="C259" s="1">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D259" s="9"/>
       <c r="E259" s="9"/>
@@ -4143,7 +4203,7 @@
       <c r="A260" s="1"/>
       <c r="B260" s="1"/>
       <c r="C260" s="1">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D260" s="9"/>
       <c r="E260" s="9"/>
@@ -4157,7 +4217,7 @@
       <c r="A261" s="1"/>
       <c r="B261" s="1"/>
       <c r="C261" s="1">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D261" s="9"/>
       <c r="E261" s="9"/>
@@ -4171,7 +4231,7 @@
       <c r="A262" s="1"/>
       <c r="B262" s="1"/>
       <c r="C262" s="1">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D262" s="9"/>
       <c r="E262" s="9"/>
@@ -4185,7 +4245,7 @@
       <c r="A263" s="1"/>
       <c r="B263" s="1"/>
       <c r="C263" s="1">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D263" s="9"/>
       <c r="E263" s="9"/>
@@ -4199,7 +4259,7 @@
       <c r="A264" s="1"/>
       <c r="B264" s="1"/>
       <c r="C264" s="1">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D264" s="9"/>
       <c r="E264" s="9"/>
@@ -4213,7 +4273,7 @@
       <c r="A265" s="1"/>
       <c r="B265" s="1"/>
       <c r="C265" s="1">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D265" s="9"/>
       <c r="E265" s="9"/>
@@ -4227,7 +4287,7 @@
       <c r="A266" s="1"/>
       <c r="B266" s="1"/>
       <c r="C266" s="1">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D266" s="9"/>
       <c r="E266" s="9"/>
@@ -4241,7 +4301,7 @@
       <c r="A267" s="1"/>
       <c r="B267" s="1"/>
       <c r="C267" s="1">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D267" s="9"/>
       <c r="E267" s="9"/>
@@ -4255,7 +4315,7 @@
       <c r="A268" s="1"/>
       <c r="B268" s="1"/>
       <c r="C268" s="1">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D268" s="9"/>
       <c r="E268" s="9"/>
@@ -4269,7 +4329,7 @@
       <c r="A269" s="1"/>
       <c r="B269" s="1"/>
       <c r="C269" s="1">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D269" s="9"/>
       <c r="E269" s="9"/>
@@ -4283,7 +4343,7 @@
       <c r="A270" s="1"/>
       <c r="B270" s="1"/>
       <c r="C270" s="1">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D270" s="9"/>
       <c r="E270" s="9"/>
@@ -4297,7 +4357,7 @@
       <c r="A271" s="1"/>
       <c r="B271" s="1"/>
       <c r="C271" s="1">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D271" s="9"/>
       <c r="E271" s="9"/>
@@ -4311,7 +4371,7 @@
       <c r="A272" s="1"/>
       <c r="B272" s="1"/>
       <c r="C272" s="1">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D272" s="9"/>
       <c r="E272" s="9"/>
@@ -4325,7 +4385,7 @@
       <c r="A273" s="1"/>
       <c r="B273" s="1"/>
       <c r="C273" s="1">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D273" s="9"/>
       <c r="E273" s="9"/>
@@ -4339,7 +4399,7 @@
       <c r="A274" s="1"/>
       <c r="B274" s="1"/>
       <c r="C274" s="1">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D274" s="9"/>
       <c r="E274" s="9"/>
@@ -4353,7 +4413,7 @@
       <c r="A275" s="1"/>
       <c r="B275" s="1"/>
       <c r="C275" s="1">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D275" s="9"/>
       <c r="E275" s="9"/>
@@ -4367,7 +4427,7 @@
       <c r="A276" s="1"/>
       <c r="B276" s="1"/>
       <c r="C276" s="1">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D276" s="9"/>
       <c r="E276" s="9"/>
@@ -4381,7 +4441,7 @@
       <c r="A277" s="1"/>
       <c r="B277" s="1"/>
       <c r="C277" s="1">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D277" s="9"/>
       <c r="E277" s="9"/>
@@ -4395,7 +4455,7 @@
       <c r="A278" s="1"/>
       <c r="B278" s="1"/>
       <c r="C278" s="1">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D278" s="9"/>
       <c r="E278" s="9"/>
@@ -4409,7 +4469,7 @@
       <c r="A279" s="1"/>
       <c r="B279" s="1"/>
       <c r="C279" s="1">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D279" s="9"/>
       <c r="E279" s="9"/>
@@ -4423,7 +4483,7 @@
       <c r="A280" s="1"/>
       <c r="B280" s="1"/>
       <c r="C280" s="1">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D280" s="9"/>
       <c r="E280" s="9"/>
@@ -4437,7 +4497,7 @@
       <c r="A281" s="1"/>
       <c r="B281" s="1"/>
       <c r="C281" s="1">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D281" s="9"/>
       <c r="E281" s="9"/>
@@ -4451,7 +4511,7 @@
       <c r="A282" s="1"/>
       <c r="B282" s="1"/>
       <c r="C282" s="1">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D282" s="9"/>
       <c r="E282" s="9"/>
@@ -4465,7 +4525,7 @@
       <c r="A283" s="1"/>
       <c r="B283" s="1"/>
       <c r="C283" s="1">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D283" s="9"/>
       <c r="E283" s="9"/>
@@ -4479,7 +4539,7 @@
       <c r="A284" s="1"/>
       <c r="B284" s="1"/>
       <c r="C284" s="1">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D284" s="9"/>
       <c r="E284" s="9"/>
@@ -4493,7 +4553,7 @@
       <c r="A285" s="1"/>
       <c r="B285" s="1"/>
       <c r="C285" s="1">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D285" s="9"/>
       <c r="E285" s="9"/>
@@ -4507,7 +4567,7 @@
       <c r="A286" s="1"/>
       <c r="B286" s="1"/>
       <c r="C286" s="1">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D286" s="9"/>
       <c r="E286" s="9"/>
@@ -4521,7 +4581,7 @@
       <c r="A287" s="1"/>
       <c r="B287" s="1"/>
       <c r="C287" s="1">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D287" s="9"/>
       <c r="E287" s="9"/>
@@ -4535,7 +4595,7 @@
       <c r="A288" s="1"/>
       <c r="B288" s="1"/>
       <c r="C288" s="1">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D288" s="9"/>
       <c r="E288" s="9"/>
@@ -4549,7 +4609,7 @@
       <c r="A289" s="1"/>
       <c r="B289" s="1"/>
       <c r="C289" s="1">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D289" s="9"/>
       <c r="E289" s="9"/>
@@ -4563,7 +4623,7 @@
       <c r="A290" s="1"/>
       <c r="B290" s="1"/>
       <c r="C290" s="1">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D290" s="9"/>
       <c r="E290" s="9"/>
@@ -4577,7 +4637,7 @@
       <c r="A291" s="1"/>
       <c r="B291" s="1"/>
       <c r="C291" s="1">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D291" s="9"/>
       <c r="E291" s="9"/>
@@ -4591,7 +4651,7 @@
       <c r="A292" s="1"/>
       <c r="B292" s="1"/>
       <c r="C292" s="1">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D292" s="9"/>
       <c r="E292" s="9"/>
@@ -4605,7 +4665,7 @@
       <c r="A293" s="1"/>
       <c r="B293" s="1"/>
       <c r="C293" s="1">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D293" s="9"/>
       <c r="E293" s="9"/>
@@ -4619,7 +4679,7 @@
       <c r="A294" s="1"/>
       <c r="B294" s="1"/>
       <c r="C294" s="1">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D294" s="9"/>
       <c r="E294" s="9"/>
@@ -4633,7 +4693,7 @@
       <c r="A295" s="1"/>
       <c r="B295" s="1"/>
       <c r="C295" s="1">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D295" s="9"/>
       <c r="E295" s="9"/>
@@ -4647,7 +4707,7 @@
       <c r="A296" s="1"/>
       <c r="B296" s="1"/>
       <c r="C296" s="1">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D296" s="9"/>
       <c r="E296" s="9"/>
@@ -4661,7 +4721,7 @@
       <c r="A297" s="1"/>
       <c r="B297" s="1"/>
       <c r="C297" s="1">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D297" s="9"/>
       <c r="E297" s="9"/>
@@ -4675,7 +4735,7 @@
       <c r="A298" s="1"/>
       <c r="B298" s="1"/>
       <c r="C298" s="1">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D298" s="9"/>
       <c r="E298" s="9"/>
@@ -4689,7 +4749,7 @@
       <c r="A299" s="1"/>
       <c r="B299" s="1"/>
       <c r="C299" s="1">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D299" s="9"/>
       <c r="E299" s="9"/>
@@ -4703,7 +4763,7 @@
       <c r="A300" s="1"/>
       <c r="B300" s="1"/>
       <c r="C300" s="1">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D300" s="9"/>
       <c r="E300" s="9"/>
@@ -4717,7 +4777,7 @@
       <c r="A301" s="1"/>
       <c r="B301" s="1"/>
       <c r="C301" s="1">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D301" s="9"/>
       <c r="E301" s="9"/>
@@ -4731,7 +4791,7 @@
       <c r="A302" s="1"/>
       <c r="B302" s="1"/>
       <c r="C302" s="1">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D302" s="9"/>
       <c r="E302" s="9"/>
@@ -4745,7 +4805,7 @@
       <c r="A303" s="1"/>
       <c r="B303" s="1"/>
       <c r="C303" s="1">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D303" s="9"/>
       <c r="E303" s="9"/>
@@ -4759,7 +4819,7 @@
       <c r="A304" s="1"/>
       <c r="B304" s="1"/>
       <c r="C304" s="1">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D304" s="9"/>
       <c r="E304" s="9"/>
@@ -4773,7 +4833,7 @@
       <c r="A305" s="1"/>
       <c r="B305" s="1"/>
       <c r="C305" s="1">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D305" s="9"/>
       <c r="E305" s="9"/>
@@ -4787,7 +4847,7 @@
       <c r="A306" s="1"/>
       <c r="B306" s="1"/>
       <c r="C306" s="1">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D306" s="9"/>
       <c r="E306" s="9"/>
@@ -4801,7 +4861,7 @@
       <c r="A307" s="1"/>
       <c r="B307" s="1"/>
       <c r="C307" s="1">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D307" s="9"/>
       <c r="E307" s="9"/>
@@ -4815,7 +4875,7 @@
       <c r="A308" s="1"/>
       <c r="B308" s="1"/>
       <c r="C308" s="1">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D308" s="9"/>
       <c r="E308" s="9"/>
@@ -4829,7 +4889,7 @@
       <c r="A309" s="1"/>
       <c r="B309" s="1"/>
       <c r="C309" s="1">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D309" s="9"/>
       <c r="E309" s="9"/>
@@ -4843,7 +4903,7 @@
       <c r="A310" s="1"/>
       <c r="B310" s="1"/>
       <c r="C310" s="1">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D310" s="9"/>
       <c r="E310" s="9"/>
@@ -4857,7 +4917,7 @@
       <c r="A311" s="1"/>
       <c r="B311" s="1"/>
       <c r="C311" s="1">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D311" s="9"/>
       <c r="E311" s="9"/>
@@ -4871,7 +4931,7 @@
       <c r="A312" s="1"/>
       <c r="B312" s="1"/>
       <c r="C312" s="1">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D312" s="9"/>
       <c r="E312" s="9"/>
@@ -4885,7 +4945,7 @@
       <c r="A313" s="1"/>
       <c r="B313" s="1"/>
       <c r="C313" s="1">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D313" s="9"/>
       <c r="E313" s="9"/>
@@ -4899,7 +4959,7 @@
       <c r="A314" s="1"/>
       <c r="B314" s="1"/>
       <c r="C314" s="1">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D314" s="9"/>
       <c r="E314" s="9"/>
@@ -4913,7 +4973,7 @@
       <c r="A315" s="1"/>
       <c r="B315" s="1"/>
       <c r="C315" s="1">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D315" s="9"/>
       <c r="E315" s="9"/>
@@ -4927,7 +4987,7 @@
       <c r="A316" s="1"/>
       <c r="B316" s="1"/>
       <c r="C316" s="1">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D316" s="9"/>
       <c r="E316" s="9"/>
@@ -4941,7 +5001,7 @@
       <c r="A317" s="1"/>
       <c r="B317" s="1"/>
       <c r="C317" s="1">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D317" s="9"/>
       <c r="E317" s="9"/>
@@ -4955,7 +5015,7 @@
       <c r="A318" s="1"/>
       <c r="B318" s="1"/>
       <c r="C318" s="1">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D318" s="9"/>
       <c r="E318" s="9"/>
@@ -4969,7 +5029,7 @@
       <c r="A319" s="1"/>
       <c r="B319" s="1"/>
       <c r="C319" s="1">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D319" s="9"/>
       <c r="E319" s="9"/>
@@ -4983,7 +5043,7 @@
       <c r="A320" s="1"/>
       <c r="B320" s="1"/>
       <c r="C320" s="1">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D320" s="9"/>
       <c r="E320" s="9"/>
@@ -4997,7 +5057,7 @@
       <c r="A321" s="1"/>
       <c r="B321" s="1"/>
       <c r="C321" s="1">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D321" s="9"/>
       <c r="E321" s="9"/>
@@ -5011,7 +5071,7 @@
       <c r="A322" s="1"/>
       <c r="B322" s="1"/>
       <c r="C322" s="1">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D322" s="9"/>
       <c r="E322" s="9"/>
@@ -5025,7 +5085,7 @@
       <c r="A323" s="1"/>
       <c r="B323" s="1"/>
       <c r="C323" s="1">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D323" s="9"/>
       <c r="E323" s="9"/>
@@ -5039,7 +5099,7 @@
       <c r="A324" s="1"/>
       <c r="B324" s="1"/>
       <c r="C324" s="1">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D324" s="9"/>
       <c r="E324" s="9"/>
@@ -5053,7 +5113,7 @@
       <c r="A325" s="1"/>
       <c r="B325" s="1"/>
       <c r="C325" s="1">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D325" s="9"/>
       <c r="E325" s="9"/>
@@ -5067,7 +5127,7 @@
       <c r="A326" s="1"/>
       <c r="B326" s="1"/>
       <c r="C326" s="1">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D326" s="9"/>
       <c r="E326" s="9"/>
@@ -5081,7 +5141,7 @@
       <c r="A327" s="1"/>
       <c r="B327" s="1"/>
       <c r="C327" s="1">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D327" s="9"/>
       <c r="E327" s="9"/>
@@ -5095,7 +5155,7 @@
       <c r="A328" s="1"/>
       <c r="B328" s="1"/>
       <c r="C328" s="1">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D328" s="9"/>
       <c r="E328" s="9"/>
@@ -5109,7 +5169,7 @@
       <c r="A329" s="1"/>
       <c r="B329" s="1"/>
       <c r="C329" s="1">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D329" s="9"/>
       <c r="E329" s="9"/>
@@ -5123,7 +5183,7 @@
       <c r="A330" s="1"/>
       <c r="B330" s="1"/>
       <c r="C330" s="1">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D330" s="9"/>
       <c r="E330" s="9"/>
@@ -5137,7 +5197,7 @@
       <c r="A331" s="1"/>
       <c r="B331" s="1"/>
       <c r="C331" s="1">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D331" s="9"/>
       <c r="E331" s="9"/>
@@ -5151,7 +5211,7 @@
       <c r="A332" s="1"/>
       <c r="B332" s="1"/>
       <c r="C332" s="1">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D332" s="9"/>
       <c r="E332" s="9"/>
@@ -5165,7 +5225,7 @@
       <c r="A333" s="1"/>
       <c r="B333" s="1"/>
       <c r="C333" s="1">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D333" s="9"/>
       <c r="E333" s="9"/>
@@ -5179,7 +5239,7 @@
       <c r="A334" s="1"/>
       <c r="B334" s="1"/>
       <c r="C334" s="1">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D334" s="9"/>
       <c r="E334" s="9"/>
@@ -5193,7 +5253,7 @@
       <c r="A335" s="1"/>
       <c r="B335" s="1"/>
       <c r="C335" s="1">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D335" s="9"/>
       <c r="E335" s="9"/>
@@ -5207,7 +5267,7 @@
       <c r="A336" s="1"/>
       <c r="B336" s="1"/>
       <c r="C336" s="1">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D336" s="9"/>
       <c r="E336" s="9"/>
@@ -5221,7 +5281,7 @@
       <c r="A337" s="1"/>
       <c r="B337" s="1"/>
       <c r="C337" s="1">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D337" s="9"/>
       <c r="E337" s="9"/>
@@ -5235,7 +5295,7 @@
       <c r="A338" s="1"/>
       <c r="B338" s="1"/>
       <c r="C338" s="1">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D338" s="9"/>
       <c r="E338" s="9"/>
@@ -5249,7 +5309,7 @@
       <c r="A339" s="1"/>
       <c r="B339" s="1"/>
       <c r="C339" s="1">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D339" s="9"/>
       <c r="E339" s="9"/>
@@ -5263,7 +5323,7 @@
       <c r="A340" s="1"/>
       <c r="B340" s="1"/>
       <c r="C340" s="1">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D340" s="9"/>
       <c r="E340" s="9"/>
@@ -5277,7 +5337,7 @@
       <c r="A341" s="1"/>
       <c r="B341" s="1"/>
       <c r="C341" s="1">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D341" s="9"/>
       <c r="E341" s="9"/>
@@ -5291,7 +5351,7 @@
       <c r="A342" s="1"/>
       <c r="B342" s="1"/>
       <c r="C342" s="1">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D342" s="9"/>
       <c r="E342" s="9"/>
@@ -5305,7 +5365,7 @@
       <c r="A343" s="1"/>
       <c r="B343" s="1"/>
       <c r="C343" s="1">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D343" s="9"/>
       <c r="E343" s="9"/>
@@ -5319,7 +5379,7 @@
       <c r="A344" s="1"/>
       <c r="B344" s="1"/>
       <c r="C344" s="1">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D344" s="9"/>
       <c r="E344" s="9"/>
@@ -5333,7 +5393,7 @@
       <c r="A345" s="1"/>
       <c r="B345" s="1"/>
       <c r="C345" s="1">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D345" s="9"/>
       <c r="E345" s="9"/>
@@ -5347,7 +5407,7 @@
       <c r="A346" s="1"/>
       <c r="B346" s="1"/>
       <c r="C346" s="1">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D346" s="9"/>
       <c r="E346" s="9"/>
@@ -5361,7 +5421,7 @@
       <c r="A347" s="1"/>
       <c r="B347" s="1"/>
       <c r="C347" s="1">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D347" s="9"/>
       <c r="E347" s="9"/>
@@ -5375,7 +5435,7 @@
       <c r="A348" s="1"/>
       <c r="B348" s="1"/>
       <c r="C348" s="1">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D348" s="9"/>
       <c r="E348" s="9"/>
@@ -5389,7 +5449,7 @@
       <c r="A349" s="1"/>
       <c r="B349" s="1"/>
       <c r="C349" s="1">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D349" s="9"/>
       <c r="E349" s="9"/>
@@ -5403,7 +5463,7 @@
       <c r="A350" s="1"/>
       <c r="B350" s="1"/>
       <c r="C350" s="1">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D350" s="9"/>
       <c r="E350" s="9"/>
@@ -5417,7 +5477,7 @@
       <c r="A351" s="1"/>
       <c r="B351" s="1"/>
       <c r="C351" s="1">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D351" s="9"/>
       <c r="E351" s="9"/>
@@ -5431,7 +5491,7 @@
       <c r="A352" s="1"/>
       <c r="B352" s="1"/>
       <c r="C352" s="1">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D352" s="9"/>
       <c r="E352" s="9"/>
@@ -5445,7 +5505,7 @@
       <c r="A353" s="1"/>
       <c r="B353" s="1"/>
       <c r="C353" s="1">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D353" s="9"/>
       <c r="E353" s="9"/>
@@ -5459,7 +5519,7 @@
       <c r="A354" s="1"/>
       <c r="B354" s="1"/>
       <c r="C354" s="1">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D354" s="9"/>
       <c r="E354" s="9"/>
@@ -5473,7 +5533,7 @@
       <c r="A355" s="1"/>
       <c r="B355" s="1"/>
       <c r="C355" s="1">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D355" s="9"/>
       <c r="E355" s="9"/>
@@ -5487,7 +5547,7 @@
       <c r="A356" s="1"/>
       <c r="B356" s="1"/>
       <c r="C356" s="1">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D356" s="9"/>
       <c r="E356" s="9"/>
@@ -5501,7 +5561,7 @@
       <c r="A357" s="1"/>
       <c r="B357" s="1"/>
       <c r="C357" s="1">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D357" s="9"/>
       <c r="E357" s="9"/>
@@ -5515,7 +5575,7 @@
       <c r="A358" s="1"/>
       <c r="B358" s="1"/>
       <c r="C358" s="1">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D358" s="9"/>
       <c r="E358" s="9"/>
@@ -5529,7 +5589,7 @@
       <c r="A359" s="1"/>
       <c r="B359" s="1"/>
       <c r="C359" s="1">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D359" s="9"/>
       <c r="E359" s="9"/>
@@ -5543,7 +5603,7 @@
       <c r="A360" s="1"/>
       <c r="B360" s="1"/>
       <c r="C360" s="1">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D360" s="9"/>
       <c r="E360" s="9"/>
@@ -5557,7 +5617,7 @@
       <c r="A361" s="1"/>
       <c r="B361" s="1"/>
       <c r="C361" s="1">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D361" s="9"/>
       <c r="E361" s="9"/>
@@ -5571,7 +5631,7 @@
       <c r="A362" s="1"/>
       <c r="B362" s="1"/>
       <c r="C362" s="1">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D362" s="9"/>
       <c r="E362" s="9"/>
@@ -5585,7 +5645,7 @@
       <c r="A363" s="1"/>
       <c r="B363" s="1"/>
       <c r="C363" s="1">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D363" s="9"/>
       <c r="E363" s="9"/>
@@ -5599,7 +5659,7 @@
       <c r="A364" s="1"/>
       <c r="B364" s="1"/>
       <c r="C364" s="1">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D364" s="9"/>
       <c r="E364" s="9"/>
@@ -5613,7 +5673,7 @@
       <c r="A365" s="1"/>
       <c r="B365" s="1"/>
       <c r="C365" s="1">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="D365" s="9"/>
       <c r="E365" s="9"/>
@@ -5627,7 +5687,7 @@
       <c r="A366" s="1"/>
       <c r="B366" s="1"/>
       <c r="C366" s="1">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D366" s="9"/>
       <c r="E366" s="9"/>
@@ -5641,7 +5701,7 @@
       <c r="A367" s="1"/>
       <c r="B367" s="1"/>
       <c r="C367" s="1">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D367" s="9"/>
       <c r="E367" s="9"/>
@@ -5655,7 +5715,7 @@
       <c r="A368" s="1"/>
       <c r="B368" s="1"/>
       <c r="C368" s="1">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D368" s="9"/>
       <c r="E368" s="9"/>
@@ -5669,7 +5729,7 @@
       <c r="A369" s="1"/>
       <c r="B369" s="1"/>
       <c r="C369" s="1">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D369" s="9"/>
       <c r="E369" s="9"/>
@@ -5683,7 +5743,7 @@
       <c r="A370" s="1"/>
       <c r="B370" s="1"/>
       <c r="C370" s="1">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D370" s="9"/>
       <c r="E370" s="9"/>
@@ -5697,7 +5757,7 @@
       <c r="A371" s="1"/>
       <c r="B371" s="1"/>
       <c r="C371" s="1">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D371" s="9"/>
       <c r="E371" s="9"/>
@@ -5711,7 +5771,7 @@
       <c r="A372" s="1"/>
       <c r="B372" s="1"/>
       <c r="C372" s="1">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D372" s="9"/>
       <c r="E372" s="9"/>
@@ -5725,7 +5785,7 @@
       <c r="A373" s="1"/>
       <c r="B373" s="1"/>
       <c r="C373" s="1">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D373" s="9"/>
       <c r="E373" s="9"/>
@@ -5739,7 +5799,7 @@
       <c r="A374" s="1"/>
       <c r="B374" s="1"/>
       <c r="C374" s="1">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D374" s="9"/>
       <c r="E374" s="9"/>
@@ -5753,7 +5813,7 @@
       <c r="A375" s="1"/>
       <c r="B375" s="1"/>
       <c r="C375" s="1">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D375" s="9"/>
       <c r="E375" s="9"/>
@@ -5767,7 +5827,7 @@
       <c r="A376" s="1"/>
       <c r="B376" s="1"/>
       <c r="C376" s="1">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D376" s="9"/>
       <c r="E376" s="9"/>
@@ -5781,7 +5841,7 @@
       <c r="A377" s="1"/>
       <c r="B377" s="1"/>
       <c r="C377" s="1">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D377" s="9"/>
       <c r="E377" s="9"/>
@@ -5795,7 +5855,7 @@
       <c r="A378" s="1"/>
       <c r="B378" s="1"/>
       <c r="C378" s="1">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D378" s="9"/>
       <c r="E378" s="9"/>
@@ -5809,7 +5869,7 @@
       <c r="A379" s="1"/>
       <c r="B379" s="1"/>
       <c r="C379" s="1">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D379" s="9"/>
       <c r="E379" s="9"/>
@@ -5823,7 +5883,7 @@
       <c r="A380" s="1"/>
       <c r="B380" s="1"/>
       <c r="C380" s="1">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D380" s="9"/>
       <c r="E380" s="9"/>
@@ -5837,7 +5897,7 @@
       <c r="A381" s="1"/>
       <c r="B381" s="1"/>
       <c r="C381" s="1">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D381" s="9"/>
       <c r="E381" s="9"/>
@@ -5851,7 +5911,7 @@
       <c r="A382" s="1"/>
       <c r="B382" s="1"/>
       <c r="C382" s="1">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D382" s="9"/>
       <c r="E382" s="9"/>
@@ -5865,7 +5925,7 @@
       <c r="A383" s="1"/>
       <c r="B383" s="1"/>
       <c r="C383" s="1">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D383" s="9"/>
       <c r="E383" s="9"/>
@@ -5879,7 +5939,7 @@
       <c r="A384" s="1"/>
       <c r="B384" s="1"/>
       <c r="C384" s="1">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D384" s="9"/>
       <c r="E384" s="9"/>
@@ -5893,7 +5953,7 @@
       <c r="A385" s="1"/>
       <c r="B385" s="1"/>
       <c r="C385" s="1">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D385" s="9"/>
       <c r="E385" s="9"/>
@@ -5907,7 +5967,7 @@
       <c r="A386" s="1"/>
       <c r="B386" s="1"/>
       <c r="C386" s="1">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D386" s="9"/>
       <c r="E386" s="9"/>
@@ -5921,7 +5981,7 @@
       <c r="A387" s="1"/>
       <c r="B387" s="1"/>
       <c r="C387" s="1">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D387" s="9"/>
       <c r="E387" s="9"/>
@@ -5935,7 +5995,7 @@
       <c r="A388" s="1"/>
       <c r="B388" s="1"/>
       <c r="C388" s="1">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D388" s="9"/>
       <c r="E388" s="9"/>
@@ -5949,7 +6009,7 @@
       <c r="A389" s="1"/>
       <c r="B389" s="1"/>
       <c r="C389" s="1">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D389" s="9"/>
       <c r="E389" s="9"/>
@@ -5963,7 +6023,7 @@
       <c r="A390" s="1"/>
       <c r="B390" s="1"/>
       <c r="C390" s="1">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D390" s="9"/>
       <c r="E390" s="9"/>
@@ -5977,7 +6037,7 @@
       <c r="A391" s="1"/>
       <c r="B391" s="1"/>
       <c r="C391" s="1">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D391" s="9"/>
       <c r="E391" s="9"/>
@@ -5991,7 +6051,7 @@
       <c r="A392" s="1"/>
       <c r="B392" s="1"/>
       <c r="C392" s="1">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D392" s="9"/>
       <c r="E392" s="9"/>
@@ -6005,7 +6065,7 @@
       <c r="A393" s="1"/>
       <c r="B393" s="1"/>
       <c r="C393" s="1">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D393" s="9"/>
       <c r="E393" s="9"/>
@@ -6019,7 +6079,7 @@
       <c r="A394" s="1"/>
       <c r="B394" s="1"/>
       <c r="C394" s="1">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D394" s="9"/>
       <c r="E394" s="9"/>
@@ -6033,7 +6093,7 @@
       <c r="A395" s="1"/>
       <c r="B395" s="1"/>
       <c r="C395" s="1">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D395" s="9"/>
       <c r="E395" s="9"/>
@@ -6047,7 +6107,7 @@
       <c r="A396" s="1"/>
       <c r="B396" s="1"/>
       <c r="C396" s="1">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D396" s="9"/>
       <c r="E396" s="9"/>
@@ -6061,7 +6121,7 @@
       <c r="A397" s="1"/>
       <c r="B397" s="1"/>
       <c r="C397" s="1">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D397" s="9"/>
       <c r="E397" s="9"/>
@@ -6075,7 +6135,7 @@
       <c r="A398" s="1"/>
       <c r="B398" s="1"/>
       <c r="C398" s="1">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D398" s="9"/>
       <c r="E398" s="9"/>
@@ -6089,7 +6149,7 @@
       <c r="A399" s="1"/>
       <c r="B399" s="1"/>
       <c r="C399" s="1">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D399" s="9"/>
       <c r="E399" s="9"/>
@@ -6103,7 +6163,7 @@
       <c r="A400" s="1"/>
       <c r="B400" s="1"/>
       <c r="C400" s="1">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D400" s="9"/>
       <c r="E400" s="9"/>
@@ -6117,7 +6177,7 @@
       <c r="A401" s="1"/>
       <c r="B401" s="1"/>
       <c r="C401" s="1">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D401" s="9"/>
       <c r="E401" s="9"/>
@@ -6131,7 +6191,7 @@
       <c r="A402" s="1"/>
       <c r="B402" s="1"/>
       <c r="C402" s="1">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D402" s="9"/>
       <c r="E402" s="9"/>
@@ -6145,7 +6205,7 @@
       <c r="A403" s="1"/>
       <c r="B403" s="1"/>
       <c r="C403" s="1">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D403" s="9"/>
       <c r="E403" s="9"/>
@@ -6159,7 +6219,7 @@
       <c r="A404" s="1"/>
       <c r="B404" s="1"/>
       <c r="C404" s="1">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D404" s="9"/>
       <c r="E404" s="9"/>
@@ -6173,7 +6233,7 @@
       <c r="A405" s="1"/>
       <c r="B405" s="1"/>
       <c r="C405" s="1">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D405" s="9"/>
       <c r="E405" s="9"/>
@@ -6187,7 +6247,7 @@
       <c r="A406" s="1"/>
       <c r="B406" s="1"/>
       <c r="C406" s="1">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D406" s="9"/>
       <c r="E406" s="9"/>
@@ -6201,7 +6261,7 @@
       <c r="A407" s="1"/>
       <c r="B407" s="1"/>
       <c r="C407" s="1">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="D407" s="9"/>
       <c r="E407" s="9"/>
@@ -6215,7 +6275,7 @@
       <c r="A408" s="1"/>
       <c r="B408" s="1"/>
       <c r="C408" s="1">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D408" s="9"/>
       <c r="E408" s="9"/>
@@ -6229,7 +6289,7 @@
       <c r="A409" s="1"/>
       <c r="B409" s="1"/>
       <c r="C409" s="1">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D409" s="9"/>
       <c r="E409" s="9"/>
@@ -6243,7 +6303,7 @@
       <c r="A410" s="1"/>
       <c r="B410" s="1"/>
       <c r="C410" s="1">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D410" s="9"/>
       <c r="E410" s="9"/>
@@ -6257,7 +6317,7 @@
       <c r="A411" s="1"/>
       <c r="B411" s="1"/>
       <c r="C411" s="1">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D411" s="9"/>
       <c r="E411" s="9"/>
@@ -6271,7 +6331,7 @@
       <c r="A412" s="1"/>
       <c r="B412" s="1"/>
       <c r="C412" s="1">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D412" s="9"/>
       <c r="E412" s="9"/>
@@ -6285,7 +6345,7 @@
       <c r="A413" s="1"/>
       <c r="B413" s="1"/>
       <c r="C413" s="1">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D413" s="9"/>
       <c r="E413" s="9"/>
@@ -6299,7 +6359,7 @@
       <c r="A414" s="1"/>
       <c r="B414" s="1"/>
       <c r="C414" s="1">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D414" s="9"/>
       <c r="E414" s="9"/>
@@ -6313,7 +6373,7 @@
       <c r="A415" s="1"/>
       <c r="B415" s="1"/>
       <c r="C415" s="1">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D415" s="9"/>
       <c r="E415" s="9"/>
@@ -6327,7 +6387,7 @@
       <c r="A416" s="1"/>
       <c r="B416" s="1"/>
       <c r="C416" s="1">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="D416" s="9"/>
       <c r="E416" s="9"/>
@@ -6341,7 +6401,7 @@
       <c r="A417" s="1"/>
       <c r="B417" s="1"/>
       <c r="C417" s="1">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D417" s="9"/>
       <c r="E417" s="9"/>
@@ -6355,7 +6415,7 @@
       <c r="A418" s="1"/>
       <c r="B418" s="1"/>
       <c r="C418" s="1">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D418" s="9"/>
       <c r="E418" s="9"/>
@@ -6369,7 +6429,7 @@
       <c r="A419" s="1"/>
       <c r="B419" s="1"/>
       <c r="C419" s="1">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D419" s="9"/>
       <c r="E419" s="9"/>
@@ -6383,7 +6443,7 @@
       <c r="A420" s="1"/>
       <c r="B420" s="1"/>
       <c r="C420" s="1">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D420" s="9"/>
       <c r="E420" s="9"/>
@@ -6397,7 +6457,7 @@
       <c r="A421" s="1"/>
       <c r="B421" s="1"/>
       <c r="C421" s="1">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D421" s="9"/>
       <c r="E421" s="9"/>
@@ -6407,33 +6467,29 @@
       <c r="I421" s="1"/>
       <c r="J421" s="1"/>
     </row>
+    <row r="422" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A422" s="1"/>
+      <c r="B422" s="1"/>
+      <c r="C422" s="1">
+        <v>420</v>
+      </c>
+      <c r="D422" s="9"/>
+      <c r="E422" s="9"/>
+      <c r="F422" s="9"/>
+      <c r="G422" s="6"/>
+      <c r="H422" s="9"/>
+      <c r="I422" s="1"/>
+      <c r="J422" s="1"/>
+    </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2 A1">
+  <dataValidations disablePrompts="1" count="1">
+    <dataValidation type="date" showInputMessage="1" showErrorMessage="1" sqref="A2:A3 A1">
       <formula1>43831</formula1>
       <formula2>44196</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967294" verticalDpi="4294967294" r:id="rId1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Лист2!$A$1:$A$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>H2:H455</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Лист2!$C$1:$C$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>J2:J456</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -6450,31 +6506,31 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C4" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>